<commit_message>
developed "David" AI some, still not very good
</commit_message>
<xml_diff>
--- a/public/spanish_03_just_lowercase no reps 10 and up.xlsx
+++ b/public/spanish_03_just_lowercase no reps 10 and up.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericw\progs\react-word-guessing-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5AAB05-76ED-4567-BA7D-AEBF25B7BB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0287274-A3B1-4E01-8706-3EC2DAE8883D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4691,7 +4691,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4883,6 +4883,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -5044,11 +5050,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5406,8 +5413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1347" workbookViewId="0">
-      <selection activeCell="K1360" sqref="K1360"/>
+    <sheetView tabSelected="1" topLeftCell="A1479" workbookViewId="0">
+      <selection activeCell="D1483" sqref="D1483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17253,50 +17260,50 @@
       </c>
     </row>
     <row r="1481" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1481" t="s">
+      <c r="A1481" s="4" t="s">
         <v>1469</v>
       </c>
-      <c r="B1481">
+      <c r="B1481" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1482" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1482" t="s">
+      <c r="A1482" s="4" t="s">
         <v>1470</v>
       </c>
-      <c r="B1482">
+      <c r="B1482" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1483" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1483" t="s">
+      <c r="A1483" s="4" t="s">
         <v>1471</v>
       </c>
-      <c r="B1483">
+      <c r="B1483" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1484" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1484" t="s">
+      <c r="A1484" s="4" t="s">
         <v>1473</v>
       </c>
-      <c r="B1484">
+      <c r="B1484" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1485" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1485" t="s">
+      <c r="A1485" s="4" t="s">
         <v>1474</v>
       </c>
-      <c r="B1485">
+      <c r="B1485" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1486" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1486" t="s">
+      <c r="A1486" s="4" t="s">
         <v>1475</v>
       </c>
-      <c r="B1486">
+      <c r="B1486" s="4">
         <v>10</v>
       </c>
     </row>
@@ -17309,58 +17316,58 @@
       </c>
     </row>
     <row r="1488" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1488" t="s">
+      <c r="A1488" s="4" t="s">
         <v>1477</v>
       </c>
-      <c r="B1488">
+      <c r="B1488" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1489" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1489" t="s">
+      <c r="A1489" s="4" t="s">
         <v>1478</v>
       </c>
-      <c r="B1489">
+      <c r="B1489" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1490" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1490" t="s">
+      <c r="A1490" s="4" t="s">
         <v>1479</v>
       </c>
-      <c r="B1490">
+      <c r="B1490" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1491" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1491" t="s">
+      <c r="A1491" s="4" t="s">
         <v>1480</v>
       </c>
-      <c r="B1491">
+      <c r="B1491" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1492" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1492" t="s">
+      <c r="A1492" s="4" t="s">
         <v>1481</v>
       </c>
-      <c r="B1492">
+      <c r="B1492" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1493" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1493" t="s">
+      <c r="A1493" s="4" t="s">
         <v>1482</v>
       </c>
-      <c r="B1493">
+      <c r="B1493" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1494" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1494" t="s">
+      <c r="A1494" s="4" t="s">
         <v>1484</v>
       </c>
-      <c r="B1494">
+      <c r="B1494" s="4">
         <v>10</v>
       </c>
     </row>
@@ -17373,10 +17380,10 @@
       </c>
     </row>
     <row r="1496" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1496" t="s">
+      <c r="A1496" s="4" t="s">
         <v>1486</v>
       </c>
-      <c r="B1496">
+      <c r="B1496" s="4">
         <v>10</v>
       </c>
     </row>
@@ -17405,18 +17412,18 @@
       </c>
     </row>
     <row r="1500" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1500" t="s">
+      <c r="A1500" s="4" t="s">
         <v>1492</v>
       </c>
-      <c r="B1500">
+      <c r="B1500" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1501" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1501" t="s">
+      <c r="A1501" s="4" t="s">
         <v>1493</v>
       </c>
-      <c r="B1501">
+      <c r="B1501" s="4">
         <v>10</v>
       </c>
     </row>
@@ -17437,10 +17444,10 @@
       </c>
     </row>
     <row r="1504" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1504" t="s">
+      <c r="A1504" s="4" t="s">
         <v>1499</v>
       </c>
-      <c r="B1504">
+      <c r="B1504" s="4">
         <v>10</v>
       </c>
     </row>
@@ -17453,18 +17460,18 @@
       </c>
     </row>
     <row r="1506" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1506" t="s">
+      <c r="A1506" s="4" t="s">
         <v>1501</v>
       </c>
-      <c r="B1506">
+      <c r="B1506" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="1507" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1507" t="s">
+      <c r="A1507" s="4" t="s">
         <v>1504</v>
       </c>
-      <c r="B1507">
+      <c r="B1507" s="4">
         <v>10</v>
       </c>
     </row>

</xml_diff>